<commit_message>
incluyendo objetivos y resultados
</commit_message>
<xml_diff>
--- a/Data/logins equivalentes.xlsx
+++ b/Data/logins equivalentes.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anaconda3\MeScripts\Comisiones4\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9405"/>
   </bookViews>
@@ -10,14 +15,14 @@
     <sheet name="Similar" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Similar!$A$1:$C$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Similar!$A$1:$C$123</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="308">
   <si>
     <t>EENN Y CONSULTORES Regiones</t>
   </si>
@@ -409,9 +414,6 @@
     <t>JNARURE3</t>
   </si>
   <si>
-    <t>JNARUSE3</t>
-  </si>
-  <si>
     <t>LUIS CHACON</t>
   </si>
   <si>
@@ -727,9 +729,6 @@
     <t>BAUGUSTO</t>
   </si>
   <si>
-    <t>AGOMEZ</t>
-  </si>
-  <si>
     <t>JTORRES</t>
   </si>
   <si>
@@ -751,9 +750,6 @@
     <t>DGISTAU</t>
   </si>
   <si>
-    <t>JEVALDIVIA</t>
-  </si>
-  <si>
     <t>SLOPEZ</t>
   </si>
   <si>
@@ -938,6 +934,18 @@
   </si>
   <si>
     <t>DHUARCAYA</t>
+  </si>
+  <si>
+    <t>JNARUSE</t>
+  </si>
+  <si>
+    <t>AOLAZABAL</t>
+  </si>
+  <si>
+    <t>JVALDIVIA</t>
+  </si>
+  <si>
+    <t>Sur (M.Guerra)</t>
   </si>
 </sst>
 </file>
@@ -945,8 +953,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1438,8 +1446,8 @@
   <cellStyleXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1498,7 +1506,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1545,59 +1553,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="88">
-    <cellStyle name="20% - Accent1" xfId="22" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="61"/>
-    <cellStyle name="20% - Accent2" xfId="26" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent2 2" xfId="62"/>
-    <cellStyle name="20% - Accent3" xfId="30" builtinId="38" customBuiltin="1"/>
     <cellStyle name="20% - Accent3 2" xfId="63"/>
-    <cellStyle name="20% - Accent4" xfId="34" builtinId="42" customBuiltin="1"/>
     <cellStyle name="20% - Accent4 2" xfId="64"/>
-    <cellStyle name="20% - Accent5" xfId="38" builtinId="46" customBuiltin="1"/>
     <cellStyle name="20% - Accent5 2" xfId="65"/>
-    <cellStyle name="20% - Accent6" xfId="42" builtinId="50" customBuiltin="1"/>
     <cellStyle name="20% - Accent6 2" xfId="66"/>
-    <cellStyle name="40% - Accent1" xfId="23" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="22" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="26" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="30" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="34" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="38" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="42" builtinId="50" customBuiltin="1"/>
     <cellStyle name="40% - Accent1 2" xfId="67"/>
-    <cellStyle name="40% - Accent2" xfId="27" builtinId="35" customBuiltin="1"/>
     <cellStyle name="40% - Accent2 2" xfId="68"/>
-    <cellStyle name="40% - Accent3" xfId="31" builtinId="39" customBuiltin="1"/>
     <cellStyle name="40% - Accent3 2" xfId="69"/>
-    <cellStyle name="40% - Accent4" xfId="35" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent4 2" xfId="70"/>
-    <cellStyle name="40% - Accent5" xfId="39" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent5 2" xfId="71"/>
-    <cellStyle name="40% - Accent6" xfId="43" builtinId="51" customBuiltin="1"/>
     <cellStyle name="40% - Accent6 2" xfId="72"/>
-    <cellStyle name="60% - Accent1" xfId="24" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="28" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="32" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="36" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="40" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="44" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="21" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="25" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="29" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="33" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="37" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="41" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="10" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="14" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="23" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="27" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="31" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="35" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="39" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="43" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="24" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="28" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="32" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="36" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="40" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="44" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Buena" xfId="9" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="14" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cancel" xfId="46"/>
     <cellStyle name="Cancel 2" xfId="47"/>
     <cellStyle name="Cancel 3" xfId="77"/>
-    <cellStyle name="Check Cell" xfId="16" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="16" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="15" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Comma 2" xfId="86"/>
     <cellStyle name="Currency 2" xfId="2"/>
     <cellStyle name="Currency 2 2" xfId="60"/>
-    <cellStyle name="Explanatory Text" xfId="19" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="9" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="5" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="6" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="7" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="8" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="12" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="15" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="5" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="8" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="21" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="25" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="29" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="33" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="37" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="41" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="12" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="10" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Moneda 2" xfId="3"/>
     <cellStyle name="Neutral" xfId="11" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1621,24 +1626,30 @@
     <cellStyle name="Normal 7" xfId="55"/>
     <cellStyle name="Normal 8" xfId="56"/>
     <cellStyle name="Normal 9" xfId="57"/>
-    <cellStyle name="Note" xfId="18" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="18" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Note 2" xfId="75"/>
     <cellStyle name="Note 2 2" xfId="76"/>
-    <cellStyle name="Output" xfId="13" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Percent 2" xfId="1"/>
     <cellStyle name="Percent 2 2" xfId="58"/>
     <cellStyle name="Percent 2 3" xfId="78"/>
     <cellStyle name="Percent 2 4" xfId="48"/>
     <cellStyle name="Percent 3" xfId="59"/>
-    <cellStyle name="Title" xfId="4" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="13" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="17" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="19" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="4" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="6" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="7" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="20" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="17" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1899,7 +1910,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1907,14 +1918,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B189" sqref="B189"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -1923,10 +1934,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>88</v>
@@ -1942,7 +1953,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -1966,10 +1977,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" t="s">
         <v>179</v>
-      </c>
-      <c r="B6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1990,10 +2001,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2014,10 +2025,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" t="s">
         <v>193</v>
-      </c>
-      <c r="B12" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2030,7 +2041,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
         <v>126</v>
@@ -2062,10 +2073,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" t="s">
         <v>169</v>
-      </c>
-      <c r="B18" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2086,34 +2097,34 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" t="s">
         <v>154</v>
-      </c>
-      <c r="B21" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2126,10 +2137,10 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2142,7 +2153,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B28" t="s">
         <v>14</v>
@@ -2153,7 +2164,7 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2161,7 +2172,7 @@
         <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
@@ -2198,18 +2209,18 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>198</v>
+      </c>
+      <c r="B36" t="s">
         <v>199</v>
-      </c>
-      <c r="B36" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2230,34 +2241,34 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39" t="s">
         <v>156</v>
-      </c>
-      <c r="B39" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" t="s">
         <v>197</v>
-      </c>
-      <c r="B40" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>182</v>
+      </c>
+      <c r="B41" t="s">
         <v>183</v>
-      </c>
-      <c r="B41" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>194</v>
+      </c>
+      <c r="B42" t="s">
         <v>195</v>
-      </c>
-      <c r="B42" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2294,26 +2305,26 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B48" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2334,10 +2345,10 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2366,10 +2377,10 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2398,7 +2409,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
@@ -2430,10 +2441,10 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B64" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2462,7 +2473,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B68" t="s">
         <v>4</v>
@@ -2470,10 +2481,10 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>144</v>
+      </c>
+      <c r="B69" t="s">
         <v>145</v>
-      </c>
-      <c r="B69" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2497,23 +2508,23 @@
         <v>129</v>
       </c>
       <c r="B72" t="s">
-        <v>130</v>
+        <v>304</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>177</v>
-      </c>
-      <c r="B73" t="s">
-        <v>130</v>
+        <v>176</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2526,7 +2537,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B76" t="s">
         <v>27</v>
@@ -2564,7 +2575,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>34</v>
       </c>
@@ -2572,7 +2583,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>113</v>
       </c>
@@ -2580,7 +2591,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>35</v>
       </c>
@@ -2588,7 +2599,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>1</v>
       </c>
@@ -2596,15 +2607,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B85" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>69</v>
       </c>
@@ -2612,23 +2623,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B88" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>72</v>
       </c>
@@ -2636,7 +2647,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>92</v>
       </c>
@@ -2644,15 +2655,16 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B91" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="C91" s="7"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>74</v>
       </c>
@@ -2660,7 +2672,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -2668,7 +2680,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>75</v>
       </c>
@@ -2676,7 +2688,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2684,81 +2696,81 @@
         <v>83</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B96" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>185</v>
-      </c>
-      <c r="B97" t="s">
-        <v>187</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B98" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="B99" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B100" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="B101" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="B102" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>117</v>
+        <v>43</v>
       </c>
       <c r="B103" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
@@ -2766,7 +2778,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B106" t="s">
         <v>6</v>
@@ -2774,7 +2786,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="B107" t="s">
         <v>6</v>
@@ -2782,55 +2794,55 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="B108" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="B109" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
+      <c r="A110" t="s">
+        <v>54</v>
+      </c>
+      <c r="B110" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>119</v>
-      </c>
-      <c r="B111" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="B112" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="B113" t="s">
-        <v>18</v>
+        <v>151</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="B114" t="s">
         <v>18</v>
@@ -2838,23 +2850,23 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>186</v>
+        <v>58</v>
       </c>
       <c r="B115" t="s">
-        <v>188</v>
+        <v>18</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>21</v>
+        <v>185</v>
       </c>
       <c r="B116" t="s">
-        <v>29</v>
+        <v>187</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B117" t="s">
         <v>29</v>
@@ -2862,15 +2874,15 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="B118" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="B119" t="s">
         <v>31</v>
@@ -2878,23 +2890,23 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
       <c r="B120" t="s">
-        <v>122</v>
+        <v>31</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="B122" t="s">
         <v>33</v>
@@ -2902,618 +2914,626 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>64</v>
       </c>
       <c r="B123" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>191</v>
+        <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>192</v>
+        <v>124</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="B125" t="s">
-        <v>138</v>
+        <v>191</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="B126" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>204</v>
+        <v>39</v>
       </c>
       <c r="B127" t="s">
-        <v>205</v>
+        <v>49</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B128" t="s">
-        <v>126</v>
+        <v>204</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B129" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B130" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>207</v>
+      </c>
+      <c r="B131" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>208</v>
+      </c>
+      <c r="B132" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B131" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B132" t="s">
+      <c r="B133" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>211</v>
-      </c>
-      <c r="B133" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B134" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="5" t="s">
-        <v>216</v>
+      <c r="A135" t="s">
+        <v>211</v>
       </c>
       <c r="B135" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B136" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>217</v>
-      </c>
-      <c r="B136" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B137" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B138" t="s">
-        <v>79</v>
+        <v>234</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B139" t="s">
-        <v>237</v>
+        <v>79</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B140" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B141" t="s">
-        <v>6</v>
+        <v>236</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B142" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B143" t="s">
-        <v>239</v>
+        <v>83</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B144" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B145" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B146" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B147" t="s">
-        <v>178</v>
+        <v>240</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B148" t="s">
-        <v>236</v>
+        <v>177</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B149" t="s">
-        <v>243</v>
+        <v>305</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B150" t="s">
-        <v>85</v>
+        <v>241</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B151" t="s">
-        <v>244</v>
+        <v>85</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B152" t="s">
-        <v>245</v>
+        <v>306</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B153" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B154" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B155" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B156" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B157" t="s">
-        <v>234</v>
+        <v>80</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B158" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B159" t="s">
-        <v>79</v>
+        <v>234</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B160" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B161" t="s">
-        <v>239</v>
+        <v>83</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B162" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B163" t="s">
-        <v>243</v>
+        <v>305</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B164" t="s">
-        <v>85</v>
+        <v>241</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B165" t="s">
-        <v>244</v>
+        <v>85</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B166" t="s">
-        <v>81</v>
+        <v>306</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B167" t="s">
-        <v>287</v>
+        <v>81</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B168" t="s">
-        <v>192</v>
+        <v>284</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B169" t="s">
-        <v>250</v>
+        <v>191</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B170" t="s">
-        <v>82</v>
+        <v>247</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B171" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B172" t="s">
-        <v>251</v>
+        <v>84</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B173" t="s">
-        <v>8</v>
+        <v>248</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B174" t="s">
-        <v>273</v>
+        <v>8</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B175" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B176" t="s">
-        <v>32</v>
+        <v>271</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B177" t="s">
-        <v>277</v>
+        <v>32</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B178" t="s">
-        <v>184</v>
+        <v>274</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B179" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B180" t="s">
-        <v>283</v>
+        <v>186</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B181" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>278</v>
+      </c>
+      <c r="B182" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="6" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="B182" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="B183" s="7" t="s">
-        <v>274</v>
+      <c r="B183" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>135</v>
+        <v>271</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>29</v>
+        <v>304</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>273</v>
+        <v>29</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>4</v>
+        <v>270</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>178</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="B192" t="s">
-        <v>240</v>
+        <v>293</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B193" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>300</v>
+      <c r="A194" s="7" t="s">
+        <v>296</v>
       </c>
       <c r="B194" t="s">
-        <v>283</v>
+        <v>236</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B195" t="s">
-        <v>237</v>
+        <v>280</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B196" t="s">
-        <v>298</v>
+        <v>235</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B197" t="s">
-        <v>245</v>
+        <v>295</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="8" t="s">
-        <v>305</v>
+      <c r="A198" t="s">
+        <v>300</v>
       </c>
       <c r="B198" t="s">
-        <v>107</v>
+        <v>242</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="B199" s="7" t="s">
-        <v>306</v>
+        <v>302</v>
+      </c>
+      <c r="B199" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="B200" s="7" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>